<commit_message>
Added InvalidLogin test cases
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\e2eAutomationProject\testData\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7B0825-D08C-439A-9E60-0A7AE6600098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65A3849-CE13-4089-B9D6-9A4020FA99D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>emailAddress</t>
   </si>
@@ -33,36 +33,17 @@
     <t>password</t>
   </si>
   <si>
-    <t>abstractemail@gmail.com</t>
-  </si>
-  <si>
-    <t>yilakec171@fixwap.com</t>
+    <t>caroxem662@besenica.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -84,34 +65,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -390,56 +352,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C23566EF-F661-4213-8B5A-60734E384CB7}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{996EBD3B-73C6-4843-8395-C5ED0735412A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>